<commit_message>
Notas TP8 e TP9.
</commit_message>
<xml_diff>
--- a/grupo1_notas.xlsx
+++ b/grupo1_notas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/terra/Dropbox/aulas/UFLA/2020_2/arqsw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156B6208-7645-254E-8EBF-6EAA05827C70}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB84E78D-409F-4F4D-84FC-476C0A59FBC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="19500" xr2:uid="{7A914FD5-7F0B-4F41-9884-1E0A488E24E2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>TP1</t>
   </si>
@@ -117,15 +117,42 @@
     <t>TP6</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Remodularização (os dois apresentaram)
 Django monolítico para Restful (ideia desafiadora, parabéns)
 MTV para Restful
 AST, Astor
 - Fizeram um exemplo simples mas que ilustra o processo
 - Apontou as limitações. Importante!</t>
+  </si>
+  <si>
+    <t>TP7</t>
+  </si>
+  <si>
+    <t>TP8</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>Clusterização em projetos Spring Boot
+- anlr4 a partir de python
+- sairam do Python e foram para o java.
+- KNN modificado (qual a modificação?)
+- Não entendi bem o que faz conceitualmente. Isso tem que melhorar nos próximos TPs.
+- clusterização a partir de dados principais (importações, etc.)
+- Perdeu muito tempo com explicação do código, mas faltou entender o que de fato está fazendo. No final falou repository, service, controller, model...
+- Limitação forte do @Entity, mas entendo.</t>
+  </si>
+  <si>
+    <t>TP9</t>
+  </si>
+  <si>
+    <t>Descobridor de arquitetura MVC e MVP
+- está mais para padrão arquitetural do que para descoberta arquitetural.
+- Antlr4 + java
+- Ficou muito aquém do que se espera de "descoberta arquitetural". Na verdade, muito próximo ao TP8 de vocês focado em padrão arquitetural. Obsersem que descoberta arquitetural, você quer ter uma visão global de como a aplicação funciona e não apenas enquadrar em um padrão arquitetural.
+- Lembrar de não focar tanto no código, mas na explicação teórica do que você faz. Nesse eu entendi, mas no TP8 ficou complicado.
+- Bom apontar limitações e dificuldades.</t>
   </si>
 </sst>
 </file>
@@ -216,7 +243,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -256,6 +283,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C604435-CF16-A64E-9760-CBF5D0FEE759}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +625,7 @@
       </c>
       <c r="C2" s="10">
         <f>SUM(C4:C998)</f>
-        <v>45.5</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -677,15 +707,47 @@
         <v>16</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C10" s="14">
         <v>7.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C11" s="9" t="s">
-        <v>17</v>
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="204" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="14">
+        <f>(0+6)/2</f>
+        <v>3</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="238" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="13">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>